<commit_message>
Time dependent career attrition
* Career attrition rate can now be configured to vary depending on the
  time a person is in the simulation.
</commit_message>
<xml_diff>
--- a/simParFile.xlsx
+++ b/simParFile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t xml:space="preserve">General parameters</t>
   </si>
@@ -146,7 +146,19 @@
     <t xml:space="preserve">Length of single attrition period</t>
   </si>
   <si>
+    <t xml:space="preserve">Fixed attrition rate</t>
+  </si>
+  <si>
     <t xml:space="preserve">Probability of attrition/period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attrition rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate</t>
   </si>
   <si>
     <t xml:space="preserve">Retirement parameters</t>
@@ -361,7 +373,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -372,10 +384,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0636459184865117"/>
-          <c:y val="0.0511891636478186"/>
-          <c:w val="0.902020319981315"/>
-          <c:h val="0.825169318002835"/>
+          <c:x val="0.0636385143127514"/>
+          <c:y val="0.0512133627481878"/>
+          <c:w val="0.901821622900402"/>
+          <c:h val="0.824613930034668"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -477,11 +489,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="39397906"/>
-        <c:axId val="86807982"/>
+        <c:axId val="66637479"/>
+        <c:axId val="91457073"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39397906"/>
+        <c:axId val="66637479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -516,12 +528,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86807982"/>
+        <c:crossAx val="91457073"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86807982"/>
+        <c:axId val="91457073"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,7 +577,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39397906"/>
+        <c:crossAx val="66637479"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -621,9 +633,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>144000</xdr:colOff>
+      <xdr:colOff>142920</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>55080</xdr:rowOff>
+      <xdr:rowOff>54000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -632,7 +644,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="33480" y="3161880"/>
-        <a:ext cx="3082320" cy="2285280"/>
+        <a:ext cx="3043080" cy="2284200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -652,15 +664,15 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -729,7 +741,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>250</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -778,8 +790,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,7 +858,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -931,7 +943,7 @@
       <formula>Recruitment!$B$9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:C10">
+  <conditionalFormatting sqref="A10:C10">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(Recruitment!$B$9)</formula>
     </cfRule>
@@ -982,16 +994,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,20 +1027,85 @@
       <c r="A4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="n">
         <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations count="2">
+  <conditionalFormatting sqref="A7:C7">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>Attrition!$B$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:B5">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>NOT(Attrition!$B$4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
     <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="decimal">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4" type="decimal">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4" type="list">
+      <formula1>Misc!$A$1:$A$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5" type="decimal">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -1056,19 +1133,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -1090,7 +1167,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -1101,7 +1178,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>56</v>
@@ -1151,7 +1228,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Streamlined reporting and plotting
</commit_message>
<xml_diff>
--- a/simParFile.xlsx
+++ b/simParFile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -384,10 +384,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0636156703007068"/>
-          <c:y val="0.0512214342001576"/>
-          <c:w val="0.901761111776686"/>
-          <c:h val="0.824428684003152"/>
+          <c:x val="0.0635500365230095"/>
+          <c:y val="0.0512295081967213"/>
+          <c:w val="0.90163136109082"/>
+          <c:h val="0.824243379571248"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -489,11 +489,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="30843945"/>
-        <c:axId val="68834275"/>
+        <c:axId val="60881024"/>
+        <c:axId val="20717516"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30843945"/>
+        <c:axId val="60881024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,12 +528,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68834275"/>
+        <c:crossAx val="20717516"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68834275"/>
+        <c:axId val="20717516"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +577,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30843945"/>
+        <c:crossAx val="60881024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -633,9 +633,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>142560</xdr:colOff>
+      <xdr:colOff>142200</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -644,7 +644,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="33480" y="3161880"/>
-        <a:ext cx="3004560" cy="2283840"/>
+        <a:ext cx="2956680" cy="2283480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -664,15 +664,15 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,7 +702,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -780,18 +780,18 @@
   </sheetPr>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,7 +843,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>2500</v>
+        <v>250</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -1002,8 +1002,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,8 +1133,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1228,7 +1228,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Increased functionality in recruitment
- Made recruitment more flexible such that not only adaptive recruitment
  is possible. New possibilities: fixed and random recruitment.
- Added basic attributes.
- Added code to copy simulation config to results database and to
  configure simulation from config stored in database.
</commit_message>
<xml_diff>
--- a/simParFile.xlsx
+++ b/simParFile.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Recruitment" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Attrition" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Retirement" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Misc" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Attributes" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Recruitment" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Attrition" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Retirement" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Misc" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t xml:space="preserve">General parameters</t>
   </si>
@@ -77,7 +78,7 @@
     <t xml:space="preserve">testSim</t>
   </si>
   <si>
-    <t xml:space="preserve">Personnel cap</t>
+    <t xml:space="preserve">Target personnel</t>
   </si>
   <si>
     <t xml:space="preserve">persons</t>
@@ -86,9 +87,6 @@
     <t xml:space="preserve">Sim start date</t>
   </si>
   <si>
-    <t xml:space="preserve">Sim end date</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sim length</t>
   </si>
   <si>
@@ -98,6 +96,60 @@
     <t xml:space="preserve">Number of DB commits</t>
   </si>
   <si>
+    <t xml:space="preserve">Personnel attributes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of attributes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed attribute?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed probabilities?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NonCom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function</t>
+  </si>
+  <si>
     <t xml:space="preserve">Recruitment parameters</t>
   </si>
   <si>
@@ -110,6 +162,9 @@
     <t xml:space="preserve">Test</t>
   </si>
   <si>
+    <t xml:space="preserve">Test 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Time between recruitment cycles</t>
   </si>
   <si>
@@ -119,15 +174,36 @@
     <t xml:space="preserve">Offset of cycle</t>
   </si>
   <si>
+    <t xml:space="preserve">Min recruitment</t>
+  </si>
+  <si>
     <t xml:space="preserve">Max recruitment</t>
   </si>
   <si>
+    <t xml:space="preserve">Adaptive recruitment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random recruitment</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fixed recruitment age?</t>
   </si>
   <si>
     <t xml:space="preserve">Recruitment age</t>
   </si>
   <si>
+    <t xml:space="preserve"># of recruits distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piecewise Linear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight</t>
+  </si>
+  <si>
     <t xml:space="preserve">Recruitment age distribution</t>
   </si>
   <si>
@@ -137,9 +213,6 @@
     <t xml:space="preserve">Age in years</t>
   </si>
   <si>
-    <t xml:space="preserve">Weight</t>
-  </si>
-  <si>
     <t xml:space="preserve">Attrition parameters</t>
   </si>
   <si>
@@ -153,9 +226,6 @@
   </si>
   <si>
     <t xml:space="preserve">Attrition rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Years</t>
   </si>
   <si>
     <t xml:space="preserve">Rate</t>
@@ -224,15 +294,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33FF99"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -240,8 +316,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF006600"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF006600"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF006600"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF006600"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,8 +356,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,7 +369,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -283,31 +389,32 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
       <font>
-        <name val="FreeSans"/>
+        <name val="Arial"/>
         <charset val="1"/>
         <family val="2"/>
-        <color rgb="FFB2B2B2"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -321,7 +428,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -353,7 +460,7 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF33FF99"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -384,10 +491,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0635500365230095"/>
-          <c:y val="0.0512295081967213"/>
-          <c:w val="0.90163136109082"/>
-          <c:h val="0.824243379571248"/>
+          <c:x val="0.0634586466165414"/>
+          <c:y val="0.0513103883801705"/>
+          <c:w val="0.900350877192982"/>
+          <c:h val="0.822071360909378"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -398,7 +505,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Recruitment!$C$13:$C$13</c:f>
+              <c:f>Recruitment!$C$24:$C$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -435,7 +542,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Recruitment!$B$14:$B$19</c:f>
+              <c:f>Recruitment!$B$25:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -462,7 +569,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Recruitment!$C$14:$C$19</c:f>
+              <c:f>Recruitment!$C$25:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -489,11 +596,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="60881024"/>
-        <c:axId val="20717516"/>
+        <c:axId val="38723251"/>
+        <c:axId val="35462587"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60881024"/>
+        <c:axId val="38723251"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,12 +635,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20717516"/>
+        <c:crossAx val="35462587"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="20717516"/>
+        <c:axId val="35462587"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +684,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60881024"/>
+        <c:crossAx val="38723251"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -628,14 +735,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>33480</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>45360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>142200</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>53280</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>138240</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>49320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -643,8 +750,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33480" y="3161880"/>
-        <a:ext cx="2956680" cy="2283480"/>
+        <a:off x="33480" y="4950000"/>
+        <a:ext cx="3590640" cy="2279880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -662,16 +769,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
@@ -685,7 +792,7 @@
       <c r="A3" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -693,7 +800,7 @@
       <c r="A4" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -701,8 +808,8 @@
       <c r="A5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>5000</v>
+      <c r="B5" s="3" t="n">
+        <v>25000</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -712,7 +819,7 @@
       <c r="A6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="4" t="n">
         <v>43101</v>
       </c>
     </row>
@@ -721,27 +828,18 @@
         <v>8</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>79625</v>
+        <v>100</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="n">
-        <f aca="false">YEARFRAC(B6,B7)</f>
-        <v>100</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -753,11 +851,11 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9" type="whole">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6:B7" type="date">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6" type="date">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -778,159 +876,700 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="E29" activeCellId="0" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 B8 B14 B16 B22 B24 B31 B33" type="list">
+      <formula1>Misc!$A$1:$A$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B7 B15 B23 B32" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>17</v>
+        <v>35</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>920</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>110</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>1100</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="F24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="C26" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="C28" s="2" t="n">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="F28" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
+      <c r="G28" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="2" t="n">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="n">
+      <c r="C30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="G30" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -938,34 +1577,20 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A12:C13">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>Recruitment!$B$9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10:C10">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>NOT(Recruitment!$B$9)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="7">
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6" type="decimal">
+  <dataValidations count="8">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 F6" type="decimal">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8" type="whole">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10:B12 F10:F12" type="list">
+      <formula1>Misc!$A$1:$A$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B13 F13" type="decimal">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9" type="list">
-      <formula1>Misc!$A$1:$A$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10" type="decimal">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B12" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B23 F23" type="list">
       <formula1>"Pointwise,Uniform"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -973,8 +1598,16 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7" type="decimal">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7 F7" type="decimal">
       <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8:B9 F8:F9" type="decimal">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B15 F15" type="list">
+      <formula1>"Pointwise,Uniform,Piecewise Linear"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -989,7 +1622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -997,88 +1630,88 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B3" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="4" t="n">
+        <v>52</v>
+      </c>
+      <c r="B4" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="5" t="n">
+      <c r="A5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="7" t="n">
         <v>0.02</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>32</v>
+      <c r="A7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="7" t="n">
         <v>0.02</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="7" t="n">
         <v>0.04</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="7" t="n">
         <v>-0.01</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="7" t="n">
         <v>0.01</v>
       </c>
     </row>
@@ -1120,7 +1753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1128,63 +1761,63 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4897959183673"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>67</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1215,7 +1848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1232,13 +1865,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="n">
+      <c r="A1" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Basic transition logic implemented
* Exactly what it says in the title. Basic transitions are in place.
  Transitions are from one state to another, occurring at certain
  intervals after being in the starting state for at least a set time.
</commit_message>
<xml_diff>
--- a/simParFile.xlsx
+++ b/simParFile.xlsx
@@ -5,15 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Attributes" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Recruitment" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Attrition" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Retirement" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Misc" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="States" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Transitions" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Recruitment" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Attrition" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Retirement" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Misc" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="75">
   <si>
     <t xml:space="preserve">General parameters</t>
   </si>
@@ -147,7 +149,79 @@
     <t xml:space="preserve">Vol</t>
   </si>
   <si>
-    <t xml:space="preserve">Function</t>
+    <t xml:space="preserve">Seniority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personnel states</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of states</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial state</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NonCom , Vol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State transitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of transitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior Promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time between transition tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offset of cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min time required in start state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master Promotion</t>
   </si>
   <si>
     <t xml:space="preserve">Recruitment parameters</t>
@@ -168,31 +242,13 @@
     <t xml:space="preserve">Time between recruitment cycles</t>
   </si>
   <si>
-    <t xml:space="preserve">months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offset of cycle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min recruitment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max recruitment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Adaptive recruitment</t>
   </si>
   <si>
-    <t xml:space="preserve">Random recruitment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fixed recruitment age?</t>
   </si>
   <si>
-    <t xml:space="preserve">Recruitment age</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># of recruits distribution</t>
+    <t xml:space="preserve">Pointwise</t>
   </si>
   <si>
     <t xml:space="preserve">Piecewise Linear</t>
@@ -204,9 +260,6 @@
     <t xml:space="preserve">Weight</t>
   </si>
   <si>
-    <t xml:space="preserve">Recruitment age distribution</t>
-  </si>
-  <si>
     <t xml:space="preserve">Uniform</t>
   </si>
   <si>
@@ -220,12 +273,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fixed attrition rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Probability of attrition/period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attrition rate</t>
   </si>
   <si>
     <t xml:space="preserve">Rate</t>
@@ -408,14 +455,7 @@
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
+    <dxf/>
   </dxfs>
   <colors>
     <indexedColors>
@@ -466,7 +506,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FFB2B2B2"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -480,7 +520,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -491,10 +531,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0634586466165414"/>
-          <c:y val="0.0513103883801705"/>
-          <c:w val="0.900350877192982"/>
-          <c:h val="0.822071360909378"/>
+          <c:x val="0.0634593592253013"/>
+          <c:y val="0.0513428120063191"/>
+          <c:w val="0.89996909446791"/>
+          <c:h val="0.82132701421801"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -596,11 +636,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="38723251"/>
-        <c:axId val="35462587"/>
+        <c:axId val="19037526"/>
+        <c:axId val="39433099"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="38723251"/>
+        <c:axId val="19037526"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,12 +675,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35462587"/>
+        <c:crossAx val="39433099"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35462587"/>
+        <c:axId val="39433099"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -684,7 +724,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38723251"/>
+        <c:crossAx val="19037526"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -740,9 +780,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>138240</xdr:colOff>
+      <xdr:colOff>136800</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -751,7 +791,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="33480" y="4950000"/>
-        <a:ext cx="3590640" cy="2279880"/>
+        <a:ext cx="3494160" cy="2278440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -777,8 +817,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.44897959183673"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
@@ -839,7 +879,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -876,19 +916,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -1104,7 +1144,7 @@
         <v>15</v>
       </c>
       <c r="B31" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,7 +1152,7 @@
         <v>16</v>
       </c>
       <c r="B32" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,6 +1172,22 @@
       </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1139,12 +1195,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="2">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B7 B15 B23 B32" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 B8 B14 B16 B22 B24 B31 B33" type="list">
       <formula1>Misc!$A$1:$A$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B7 B15 B23 B32" type="whole">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1163,6 +1219,435 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A20" activeCellId="0" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B7 B12 B17 B22 B27" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B8:C8 B13:C13 B18:C18 B23:C23 B28:C29" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 B11 B16 B21 B26" type="list">
+      <formula1>Misc!$A$1:$A$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:B7 B12:B14" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C10 C17" type="list">
+      <formula1>"years,months"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8 B10 B15 B17" type="decimal">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9 B16" type="decimal">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1170,86 +1655,87 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
-        <v>37</v>
+      <c r="A8" s="6" t="str">
+        <f aca="false">IF(B10,"Min recruitment","ignored")</f>
+        <v>ignored</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>92</v>
@@ -1258,8 +1744,9 @@
         <v>6</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
-        <v>37</v>
+      <c r="E8" s="6" t="str">
+        <f aca="false">IF(F10,"Min recruitment","ignored")</f>
+        <v>ignored</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>920</v>
@@ -1269,18 +1756,20 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>38</v>
+      <c r="A9" s="6" t="str">
+        <f aca="false">IF(B10,"Max recruitment",IF(B11,"ignored","Recruitment"))</f>
+        <v>Recruitment</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="6" t="s">
-        <v>38</v>
+      <c r="E9" s="6" t="str">
+        <f aca="false">IF(F10,"Max recruitment",IF(F11,"ignored","Recruitment"))</f>
+        <v>ignored</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>1100</v>
@@ -1291,27 +1780,29 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="F10" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>40</v>
+      <c r="A11" s="6" t="str">
+        <f aca="false">IF(B10,"ignored","Random recruitment")</f>
+        <v>Random recruitment</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>40</v>
+        <v>0</v>
+      </c>
+      <c r="E11" s="6" t="str">
+        <f aca="false">IF(F10,"ignored","Random recruitment")</f>
+        <v>Random recruitment</v>
       </c>
       <c r="F11" s="5" t="n">
         <v>1</v>
@@ -1319,21 +1810,22 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="F12" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>42</v>
+      <c r="A13" s="6" t="str">
+        <f aca="false">IF(B12,"Recruitment age","ignored")</f>
+        <v>ignored</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>18</v>
@@ -1342,8 +1834,9 @@
         <v>9</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="6" t="s">
-        <v>42</v>
+      <c r="E13" s="6" t="str">
+        <f aca="false">IF(F12,"Recruitment age","ignored")</f>
+        <v>ignored</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>18</v>
@@ -1353,45 +1846,47 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>43</v>
+      <c r="A15" s="6" t="str">
+        <f aca="false">IF(AND(NOT(B10),B11),"# of recruits distribution","ignored")</f>
+        <v>ignored</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
-        <v>43</v>
+      <c r="E15" s="6" t="str">
+        <f aca="false">IF(AND(NOT(F10),F11),"# of recruits distribution","ignored")</f>
+        <v># of recruits distribution</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="G15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
       <c r="B16" s="6" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>90</v>
@@ -1402,7 +1897,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="n">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
@@ -1415,12 +1910,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
       <c r="F19" s="2" t="n">
         <v>100</v>
       </c>
@@ -1429,12 +1920,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2" t="n">
-        <v>105</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
       <c r="F20" s="2" t="n">
         <v>105</v>
       </c>
@@ -1443,12 +1930,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2" t="n">
-        <v>110</v>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>2</v>
-      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
       <c r="F21" s="2" t="n">
         <v>110</v>
       </c>
@@ -1457,36 +1940,38 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>47</v>
+      <c r="A23" s="6" t="str">
+        <f aca="false">IF(B12,"ignored","Recruitment age distribution")</f>
+        <v>Recruitment age distribution</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="6" t="s">
-        <v>47</v>
+      <c r="E23" s="6" t="str">
+        <f aca="false">IF(F12,"ignored","Recruitment age distribution")</f>
+        <v>Recruitment age distribution</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="G23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6"/>
       <c r="B24" s="6" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D24" s="6"/>
       <c r="F24" s="6" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,7 +2107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1630,57 +2115,59 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B4" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>53</v>
+      <c r="A5" s="6" t="str">
+        <f aca="false">IF(B4,"Probability of attrition/period","ignored")</f>
+        <v>ignored</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>0.02</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>54</v>
+      <c r="A7" s="6" t="str">
+        <f aca="false">IF(B4,"ignored","Attrition rate")</f>
+        <v>Attrition rate</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,7 +2240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1761,49 +2248,49 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>9</v>
@@ -1811,7 +2298,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>67</v>
@@ -1848,7 +2335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>

</xml_diff>

<commit_message>
Plot of state/transition map
- Added code to make a plot of a group of states and all the transitions
  involving those states.
</commit_message>
<xml_diff>
--- a/simParFile.xlsx
+++ b/simParFile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -595,7 +595,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -606,10 +606,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0633736205990541"/>
-          <c:y val="0.0513915243516762"/>
-          <c:w val="0.899421965317919"/>
-          <c:h val="0.820208728652751"/>
+          <c:x val="0.0634663206833171"/>
+          <c:y val="0.0514077823473584"/>
+          <c:w val="0.899124229646448"/>
+          <c:h val="0.819835495096488"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -711,11 +711,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="28921347"/>
-        <c:axId val="47740609"/>
+        <c:axId val="33521932"/>
+        <c:axId val="61776969"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="28921347"/>
+        <c:axId val="33521932"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -750,12 +750,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47740609"/>
+        <c:crossAx val="61776969"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47740609"/>
+        <c:axId val="61776969"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -799,7 +799,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28921347"/>
+        <c:crossAx val="33521932"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -855,9 +855,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>134640</xdr:colOff>
+      <xdr:colOff>133920</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -866,7 +866,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="33480" y="4950000"/>
-        <a:ext cx="3425040" cy="2276280"/>
+        <a:ext cx="3329280" cy="2275560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -892,9 +892,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,7 +923,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>25000</v>
+        <v>2500</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -943,7 +942,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>9</v>
@@ -1003,8 +1002,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1306,8 +1305,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,12 +1515,12 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 B11 B16 B21 B26" type="list">
+      <formula1>Misc!$A$1:$A$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B8:C8 B13:C13 B18:C18 B23:C23 B28:C29" type="none">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 B11 B16 B21 B26" type="list">
-      <formula1>Misc!$A$1:$A$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1552,8 +1551,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,7 +1725,7 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1737,8 +1735,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1826,7 +1824,7 @@
         <v>Min recruitment</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>350</v>
+        <v>35</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>6</v>
@@ -1849,7 +1847,7 @@
         <v>Max recruitment</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>550</v>
+        <v>55</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>6</v>
@@ -1960,7 +1958,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="n">
-        <v>350</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
@@ -1974,7 +1972,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="n">
-        <v>450</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>3</v>
@@ -1988,7 +1986,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="n">
-        <v>550</v>
+        <v>55</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1</v>
@@ -2201,8 +2199,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2334,8 +2332,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2423,18 +2421,18 @@
   </sheetPr>
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2450,7 +2448,7 @@
         <v>76</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,7 +2795,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Increased versatility of transitions
- Increased the versatility of transitions. Now transitions can
  1. have a chance of occurring.
  2. occur multiple times, each time with a possibly different chance.
  3. fire personnel members if all chances of performing the transition
     have been exhausted.
  4. have a maximum number of people who can make the transition every
     period. [Max flux]
  5. set extra conditions besides initial state that need to be
     fulfilled.
  6. change extra attributes on top of the new state.
- Streamlined the transition process: instead of having a process for
  each individual personnel member, there is one process per transition
  for the system, and the process checks who's eligible for making the
  transition.
</commit_message>
<xml_diff>
--- a/simParFile.xlsx
+++ b/simParFile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="104">
   <si>
     <t xml:space="preserve">General parameters</t>
   </si>
@@ -222,7 +222,46 @@
     <t xml:space="preserve">Min time required in start state</t>
   </si>
   <si>
+    <t xml:space="preserve"># of extra conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># of extra attribute changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max # of attempts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!!! -1 for infinite, 0 for length of prob vector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forced resignation on failure?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!!! -1 for infinite</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># of transition probs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of transition probs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Master Promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experienced Promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra attribute changes</t>
   </si>
   <si>
     <t xml:space="preserve">Recruitment parameters</t>
@@ -495,11 +534,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -595,7 +634,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -606,10 +645,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0634663206833171"/>
-          <c:y val="0.0514077823473584"/>
-          <c:w val="0.899124229646448"/>
-          <c:h val="0.819835495096488"/>
+          <c:x val="0.06331241595697"/>
+          <c:y val="0.051464766429137"/>
+          <c:w val="0.898588077095473"/>
+          <c:h val="0.818527315914489"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -711,11 +750,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="33521932"/>
-        <c:axId val="61776969"/>
+        <c:axId val="90552175"/>
+        <c:axId val="33707472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33521932"/>
+        <c:axId val="90552175"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -750,12 +789,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61776969"/>
+        <c:crossAx val="33707472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61776969"/>
+        <c:axId val="33707472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -799,7 +838,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33521932"/>
+        <c:crossAx val="90552175"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -855,9 +894,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>133920</xdr:colOff>
+      <xdr:colOff>131400</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>45000</xdr:rowOff>
+      <xdr:rowOff>42480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -866,7 +905,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="33480" y="4950000"/>
-        <a:ext cx="3329280" cy="2275560"/>
+        <a:ext cx="3212280" cy="2273040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -887,13 +926,14 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,17 +1033,16 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
       <selection pane="bottomRight" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1293,20 +1332,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="bottomRight" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1320,7 +1358,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1433,7 +1471,7 @@
         <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,7 +1479,7 @@
         <v>34</v>
       </c>
       <c r="B21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1457,10 +1495,10 @@
         <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,7 +1506,7 @@
         <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,7 +1514,7 @@
         <v>34</v>
       </c>
       <c r="B26" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,7 +1522,7 @@
         <v>35</v>
       </c>
       <c r="B27" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1492,17 +1530,52 @@
         <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="2" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1511,15 +1584,15 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B7 B12 B17 B22 B27" type="whole">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B7 B12 B17 B22 B27 B32" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 B11 B16 B21 B26" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 B11 B16 B21 B26 B31" type="list">
       <formula1>Misc!$A$1:$A$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B8:C8 B13:C13 B18:C18 B23:C23 B28:C29" type="none">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B8:C8 B13:C13 B18:C18 B23:C23 B28:C28 B33:C34" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1539,19 +1612,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="D43" activeCellId="0" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1565,7 +1639,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,85 +1699,385 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>54</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>56</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B15" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>49</v>
+        <v>10</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B25" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="6" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="6" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="6" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations count="5">
+  <dataValidations count="12">
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:B7 B12:B14" type="none">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:B7 B20:B22 B35:B37" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C10 C17" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B14 B29 B46" type="list">
+      <formula1>Misc!$A$1:$A$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C10 C25 C40" type="list">
       <formula1>"years,months"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8 B10 B15 B17" type="decimal">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8 B10 B23 B25 B38 B40" type="decimal">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9 B16" type="decimal">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9 B24 B39" type="decimal">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B16 B31 B48" type="whole">
+      <formula1>1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B17:B18 B32:B33 B49" type="decimal">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B13 B15 B28 B30 B45 B47" type="whole">
+      <formula1>-1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11:B12 B26:B27 B41 B43" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C42" type="list">
+      <formula1>Misc!$C$1:$C$8</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D42 B44:C44" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1735,19 +2109,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>2</v>
@@ -1755,21 +2129,21 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>12</v>
@@ -1778,7 +2152,7 @@
         <v>49</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>12</v>
@@ -1808,74 +2182,74 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="str">
+      <c r="A8" s="7" t="str">
         <f aca="false">IF(B10,"Min recruitment","ignored")</f>
         <v>ignored</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>92</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6" t="str">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="str">
         <f aca="false">IF(F10,"Min recruitment","ignored")</f>
         <v>Min recruitment</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="str">
+      <c r="A9" s="7" t="str">
         <f aca="false">IF(B10,"Max recruitment",IF(B11,"ignored","Recruitment"))</f>
         <v>ignored</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6" t="str">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="str">
         <f aca="false">IF(F10,"Max recruitment",IF(F11,"ignored","Recruitment"))</f>
         <v>Max recruitment</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>55</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="F10" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="str">
+      <c r="A11" s="7" t="str">
         <f aca="false">IF(B10,"ignored","Random recruitment")</f>
         <v>Random recruitment</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="6" t="str">
+      <c r="E11" s="7" t="str">
         <f aca="false">IF(F10,"ignored","Random recruitment")</f>
         <v>ignored</v>
       </c>
@@ -1885,75 +2259,75 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="F12" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="str">
+      <c r="A13" s="7" t="str">
         <f aca="false">IF(B12,"Recruitment age","ignored")</f>
         <v>ignored</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6" t="str">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="str">
         <f aca="false">IF(F12,"Recruitment age","ignored")</f>
         <v>ignored</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="str">
+      <c r="A15" s="7" t="str">
         <f aca="false">IF(AND(NOT(B10),B11),"# of recruits distribution","ignored")</f>
         <v># of recruits distribution</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="str">
+        <v>74</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="str">
         <f aca="false">IF(AND(NOT(F10),F11),"# of recruits distribution","ignored")</f>
         <v>ignored</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="6"/>
+        <v>74</v>
+      </c>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>63</v>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,38 +2393,38 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="str">
+      <c r="A23" s="7" t="str">
         <f aca="false">IF(B12,"ignored","Recruitment age distribution")</f>
         <v>Recruitment age distribution</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6" t="str">
+        <v>77</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="str">
         <f aca="false">IF(F12,"ignored","Recruitment age distribution")</f>
         <v>Recruitment age distribution</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="F24" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>63</v>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="F24" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2191,27 +2565,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>12</v>
@@ -2222,63 +2596,55 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B4" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="str">
+      <c r="A5" s="7" t="str">
         <f aca="false">IF(B4,"Probability of attrition/period","ignored")</f>
         <v>ignored</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="6" t="n">
         <v>0.02</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="str">
+      <c r="A7" s="7" t="str">
         <f aca="false">IF(B4,"ignored","Attrition rate")</f>
         <v>Attrition rate</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>69</v>
+      <c r="C7" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>0.02</v>
+        <v>0</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>0.01</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>0.04</v>
+        <v>4</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>0.0075</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="C11" s="7" t="n">
-        <v>0.01</v>
+      <c r="C10" s="6" t="n">
+        <v>0.005</v>
       </c>
     </row>
   </sheetData>
@@ -2332,19 +2698,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>1</v>
@@ -2366,7 +2732,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>45</v>
@@ -2377,7 +2743,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>67</v>
@@ -2421,63 +2787,62 @@
   </sheetPr>
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="J5" s="2"/>
       <c r="M5" s="0" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>12</v>
@@ -2486,7 +2851,7 @@
         <v>49</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>12</v>
@@ -2495,7 +2860,7 @@
         <v>49</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="J6" s="3" t="n">
         <v>6</v>
@@ -2504,7 +2869,7 @@
         <v>49</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="N6" s="3" t="n">
         <v>12</v>
@@ -2515,25 +2880,25 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="F7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="J7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="N7" s="5" t="n">
         <v>1</v>
@@ -2541,25 +2906,25 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="J8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="N8" s="5" t="n">
         <v>1</v>
@@ -2567,25 +2932,25 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="F9" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="J9" s="5" t="n">
         <v>1</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="N9" s="5" t="n">
         <v>1</v>
@@ -2593,25 +2958,25 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F10" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="J10" s="5" t="n">
         <v>1</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="N10" s="5" t="n">
         <v>1</v>
@@ -2619,61 +2984,61 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="F12" s="2"/>
       <c r="I12" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="N12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="F13" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="J13" s="5" t="n">
         <v>1</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="N13" s="5" t="n">
         <v>1</v>
@@ -2681,25 +3046,25 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="J14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="N14" s="5" t="n">
         <v>1</v>
@@ -2707,25 +3072,25 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="J15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="N15" s="5" t="n">
         <v>1</v>
@@ -2733,25 +3098,25 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="J16" s="5" t="n">
         <v>1</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="N16" s="5" t="n">
         <v>1</v>
@@ -2795,7 +3160,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Target capacity of states added
- Added a target capacity for states.
- Changed the layout of the transition sheet in the Excel file.
- Added option to request network plot from Excel.
- Added option to configure simulation without running it.
    (useful for checking network)
</commit_message>
<xml_diff>
--- a/simParFile.xlsx
+++ b/simParFile.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Attributes" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="States" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Transitions" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Recruitment" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Attrition" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Retirement" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Output plots" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Misc" sheetId="9" state="hidden" r:id="rId10"/>
+    <sheet name="State Map" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Recruitment" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Attrition" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Retirement" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Output plots" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Misc" sheetId="10" state="hidden" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="110">
   <si>
     <t xml:space="preserve">General parameters</t>
   </si>
@@ -99,6 +100,9 @@
     <t xml:space="preserve">Number of DB commits</t>
   </si>
   <si>
+    <t xml:space="preserve">Run simulation?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Personnel attributes</t>
   </si>
   <si>
@@ -171,6 +175,9 @@
     <t xml:space="preserve">Initial state</t>
   </si>
   <si>
+    <t xml:space="preserve">Target # of personnel</t>
+  </si>
+  <si>
     <t xml:space="preserve"># requirements</t>
   </si>
   <si>
@@ -210,6 +217,12 @@
     <t xml:space="preserve">End state</t>
   </si>
   <si>
+    <t xml:space="preserve"># of extra conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># of extra attribute changes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Time between transition tests</t>
   </si>
   <si>
@@ -222,12 +235,6 @@
     <t xml:space="preserve">Min time required in start state</t>
   </si>
   <si>
-    <t xml:space="preserve"># of extra conditions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># of extra attribute changes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Max # of attempts</t>
   </si>
   <si>
@@ -262,6 +269,18 @@
   </si>
   <si>
     <t xml:space="preserve">Extra attribute changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plot of State Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show plot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">States to show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">States</t>
   </si>
   <si>
     <t xml:space="preserve">Recruitment parameters</t>
@@ -418,6 +437,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -435,15 +461,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,6 +473,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF33FF99"/>
         <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor rgb="FF33FF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -509,7 +540,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -530,7 +561,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -538,15 +605,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -609,7 +668,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FF66FFFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -634,7 +693,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -645,10 +704,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.06331241595697"/>
-          <c:y val="0.051464766429137"/>
-          <c:w val="0.898588077095473"/>
-          <c:h val="0.818527315914489"/>
+          <c:x val="0.0634230108757871"/>
+          <c:y val="0.0514973855173507"/>
+          <c:w val="0.898225529479107"/>
+          <c:h val="0.817778482015529"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -750,11 +809,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="90552175"/>
-        <c:axId val="33707472"/>
+        <c:axId val="19853575"/>
+        <c:axId val="442317"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90552175"/>
+        <c:axId val="19853575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -789,12 +848,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33707472"/>
+        <c:crossAx val="442317"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33707472"/>
+        <c:axId val="442317"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,7 +897,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90552175"/>
+        <c:crossAx val="19853575"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -894,9 +953,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>131400</xdr:colOff>
+      <xdr:colOff>129960</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>41040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -905,7 +964,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="33480" y="4950000"/>
-        <a:ext cx="3212280" cy="2273040"/>
+        <a:ext cx="3144240" cy="2271600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -923,15 +982,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
@@ -996,11 +1055,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="4">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10" type="list">
+      <formula1>Misc!$A$1:$A$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -1022,6 +1093,45 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="18" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1042,18 +1152,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>4</v>
@@ -1061,23 +1171,23 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>2</v>
@@ -1085,18 +1195,18 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -1104,7 +1214,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>75</v>
@@ -1112,7 +1222,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>25</v>
@@ -1120,23 +1230,23 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="B14" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3" t="n">
         <v>2</v>
@@ -1144,18 +1254,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B16" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
@@ -1163,7 +1273,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>60</v>
@@ -1171,7 +1281,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>40</v>
@@ -1179,23 +1289,23 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="B22" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B23" s="3" t="n">
         <v>3</v>
@@ -1203,18 +1313,18 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B24" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>0</v>
@@ -1222,7 +1332,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>10</v>
@@ -1230,7 +1340,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>30</v>
@@ -1238,7 +1348,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>60</v>
@@ -1246,23 +1356,23 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="B31" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B32" s="3" t="n">
         <v>2</v>
@@ -1270,18 +1380,18 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B33" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
@@ -1289,7 +1399,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>80</v>
@@ -1297,7 +1407,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>20</v>
@@ -1332,30 +1442,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>6</v>
@@ -1363,237 +1473,289 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="B6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>37</v>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="5" t="n">
-        <v>0</v>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="3" t="n">
-        <v>1</v>
+      <c r="B12" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>37</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="5" t="n">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="3" t="n">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>38</v>
+      <c r="B19" s="3" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="3" t="n">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="5" t="n">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="B30" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="5" t="n">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B32" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="2" t="s">
+      <c r="B37" s="3" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B7 B12 B17 B22 B27 B32" type="whole">
+  <dataValidations count="4">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B8 B14 B20 B26 B32 B38" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 B11 B16 B21 B26 B31" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 B12 B18 B24 B30 B36" type="list">
       <formula1>Misc!$A$1:$A$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B8:C8 B13:C13 B18:C18 B23:C23 B28:C28 B33:C34" type="none">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B9:C9 B15:C15 B21:C21 B27:C27 B33:C33 B39:C40" type="none">
       <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7 B13 B19 B25 B31 B37" type="whole">
+      <formula1>-1</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1614,29 +1776,29 @@
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="D43" activeCellId="0" sqref="D43"/>
+      <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>3</v>
@@ -1644,387 +1806,387 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>48</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>49</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="B8" s="9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="B9" s="9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
+        <v>52</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="3" t="n">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="3" t="n">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="B13" s="10" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="5" t="n">
+        <v>58</v>
+      </c>
+      <c r="B14" s="12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="3" t="n">
+        <v>59</v>
+      </c>
+      <c r="B15" s="10" t="n">
         <v>10</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="3" t="n">
+        <v>61</v>
+      </c>
+      <c r="B16" s="10" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="6" t="n">
+        <v>62</v>
+      </c>
+      <c r="B17" s="13" t="n">
         <v>0.25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="6" t="n">
+      <c r="B18" s="13" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="B23" s="9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="B24" s="9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>9</v>
+        <v>52</v>
+      </c>
+      <c r="B25" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="3" t="n">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="B26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="3" t="n">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="B27" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="B28" s="10" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="5" t="n">
+        <v>58</v>
+      </c>
+      <c r="B29" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="3" t="n">
+        <v>59</v>
+      </c>
+      <c r="B30" s="10" t="n">
         <v>10</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="3" t="n">
+        <v>61</v>
+      </c>
+      <c r="B31" s="10" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="6" t="n">
+        <v>62</v>
+      </c>
+      <c r="B32" s="13" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="6" t="n">
+      <c r="B33" s="13" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>62</v>
+        <v>46</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>48</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="B38" s="9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>49</v>
+        <v>65</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>9</v>
+      <c r="B40" s="9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" s="3" t="n">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>26</v>
+        <v>52</v>
+      </c>
+      <c r="B42" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="B43" s="3" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>25</v>
+        <v>55</v>
+      </c>
+      <c r="B44" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="B45" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="5" t="n">
+        <v>58</v>
+      </c>
+      <c r="B46" s="12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="3" t="n">
+        <v>59</v>
+      </c>
+      <c r="B47" s="10" t="n">
         <v>5</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B48" s="3" t="n">
+        <v>61</v>
+      </c>
+      <c r="B48" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B49" s="6" t="n">
+        <v>62</v>
+      </c>
+      <c r="B49" s="13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2045,15 +2207,15 @@
       <formula1>Misc!$A$1:$A$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C10 C25 C40" type="list">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C12 C27 C44" type="list">
       <formula1>"years,months"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8 B10 B23 B25 B38 B40" type="decimal">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10 B12 B25 B27 B42 B44" type="decimal">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9 B24 B39" type="decimal">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11 B26 B43" type="decimal">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2069,15 +2231,15 @@
       <formula1>-1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11:B12 B26:B27 B41 B43" type="whole">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8:B9 B23:B24 B38 B40" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C42" type="list">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C39" type="list">
       <formula1>Misc!$C$1:$C$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D42 B44:C44" type="none">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D39 B41:C41" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2097,6 +2259,94 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="list">
+      <formula1>Misc!$A$1:$A$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2109,19 +2359,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>2</v>
@@ -2129,205 +2379,205 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>6</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="str">
+      <c r="A8" s="14" t="str">
         <f aca="false">IF(B10,"Min recruitment","ignored")</f>
         <v>ignored</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>92</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="str">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="str">
         <f aca="false">IF(F10,"Min recruitment","ignored")</f>
         <v>Min recruitment</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="str">
+      <c r="A9" s="14" t="str">
         <f aca="false">IF(B10,"Max recruitment",IF(B11,"ignored","Recruitment"))</f>
         <v>ignored</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="str">
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="str">
         <f aca="false">IF(F10,"Max recruitment",IF(F11,"ignored","Recruitment"))</f>
         <v>Max recruitment</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>55</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="5" t="n">
+        <v>78</v>
+      </c>
+      <c r="B10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="5" t="n">
+        <v>78</v>
+      </c>
+      <c r="F10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="str">
+      <c r="A11" s="14" t="str">
         <f aca="false">IF(B10,"ignored","Random recruitment")</f>
         <v>Random recruitment</v>
       </c>
-      <c r="B11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7" t="str">
+      <c r="B11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14" t="str">
         <f aca="false">IF(F10,"ignored","Random recruitment")</f>
         <v>ignored</v>
       </c>
-      <c r="F11" s="5" t="n">
+      <c r="F11" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="5" t="n">
+        <v>79</v>
+      </c>
+      <c r="B12" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="5" t="n">
+        <v>79</v>
+      </c>
+      <c r="F12" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="str">
+      <c r="A13" s="14" t="str">
         <f aca="false">IF(B12,"Recruitment age","ignored")</f>
         <v>ignored</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7" t="str">
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="str">
         <f aca="false">IF(F12,"Recruitment age","ignored")</f>
         <v>ignored</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="str">
+      <c r="A15" s="14" t="str">
         <f aca="false">IF(AND(NOT(B10),B11),"# of recruits distribution","ignored")</f>
         <v># of recruits distribution</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7" t="str">
+        <v>80</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14" t="str">
         <f aca="false">IF(AND(NOT(F10),F11),"# of recruits distribution","ignored")</f>
         <v>ignored</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="7"/>
+        <v>80</v>
+      </c>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>76</v>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2393,38 +2643,38 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="str">
+      <c r="A23" s="14" t="str">
         <f aca="false">IF(B12,"ignored","Recruitment age distribution")</f>
         <v>Recruitment age distribution</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7" t="str">
+        <v>83</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14" t="str">
         <f aca="false">IF(F12,"ignored","Recruitment age distribution")</f>
         <v>Recruitment age distribution</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="F24" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>76</v>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="F24" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2516,12 +2766,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="8">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10:B12 F10:F12" type="list">
+      <formula1>Misc!$A$1:$A$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 F6" type="decimal">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10:B12 F10:F12" type="list">
-      <formula1>Misc!$A$1:$A$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B13 F13" type="decimal">
@@ -2560,7 +2810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2573,61 +2823,61 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="5" t="n">
+        <v>87</v>
+      </c>
+      <c r="B4" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="str">
+      <c r="A5" s="14" t="str">
         <f aca="false">IF(B4,"Probability of attrition/period","ignored")</f>
         <v>ignored</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="15" t="n">
         <v>0.02</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="str">
+      <c r="A7" s="14" t="str">
         <f aca="false">IF(B4,"ignored","Attrition rate")</f>
         <v>Attrition rate</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>82</v>
+      <c r="B7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="15" t="n">
         <v>0.01</v>
       </c>
     </row>
@@ -2635,7 +2885,7 @@
       <c r="B9" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="15" t="n">
         <v>0.0075</v>
       </c>
     </row>
@@ -2643,7 +2893,7 @@
       <c r="B10" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="15" t="n">
         <v>0.005</v>
       </c>
     </row>
@@ -2685,7 +2935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2698,41 +2948,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>45</v>
@@ -2743,7 +2993,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>67</v>
@@ -2780,37 +3030,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>87</v>
+      <c r="A1" s="16" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>89</v>
+      <c r="A3" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>0</v>
@@ -2818,307 +3068,307 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>0</v>
+        <v>96</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="J5" s="2"/>
       <c r="M5" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="J6" s="3" t="n">
         <v>6</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="N6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="B7" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="F7" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="J7" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="J7" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="N7" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="N7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="5" t="n">
+        <v>101</v>
+      </c>
+      <c r="B8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="5" t="n">
+        <v>101</v>
+      </c>
+      <c r="F8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="J8" s="5" t="n">
+        <v>101</v>
+      </c>
+      <c r="J8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="N8" s="5" t="n">
+        <v>101</v>
+      </c>
+      <c r="N8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="5" t="n">
+        <v>102</v>
+      </c>
+      <c r="B9" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F9" s="5" t="n">
+        <v>102</v>
+      </c>
+      <c r="F9" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="5" t="n">
+        <v>102</v>
+      </c>
+      <c r="J9" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="N9" s="5" t="n">
+        <v>102</v>
+      </c>
+      <c r="N9" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B10" s="5" t="n">
+        <v>103</v>
+      </c>
+      <c r="B10" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F10" s="5" t="n">
+        <v>103</v>
+      </c>
+      <c r="F10" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="J10" s="5" t="n">
+        <v>103</v>
+      </c>
+      <c r="J10" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="N10" s="5" t="n">
+        <v>103</v>
+      </c>
+      <c r="N10" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>98</v>
+      <c r="A11" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F12" s="2"/>
       <c r="I12" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="N12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="5" t="n">
+        <v>106</v>
+      </c>
+      <c r="B13" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="5" t="n">
+        <v>106</v>
+      </c>
+      <c r="F13" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="J13" s="5" t="n">
+        <v>106</v>
+      </c>
+      <c r="J13" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="N13" s="5" t="n">
+        <v>106</v>
+      </c>
+      <c r="N13" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="5" t="n">
+        <v>107</v>
+      </c>
+      <c r="B14" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" s="5" t="n">
+        <v>107</v>
+      </c>
+      <c r="F14" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="J14" s="5" t="n">
+        <v>107</v>
+      </c>
+      <c r="J14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="N14" s="5" t="n">
+        <v>107</v>
+      </c>
+      <c r="N14" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15" s="5" t="n">
+        <v>108</v>
+      </c>
+      <c r="B15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" s="5" t="n">
+        <v>108</v>
+      </c>
+      <c r="F15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="J15" s="5" t="n">
+        <v>108</v>
+      </c>
+      <c r="J15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="N15" s="5" t="n">
+        <v>108</v>
+      </c>
+      <c r="N15" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="5" t="n">
+        <v>109</v>
+      </c>
+      <c r="B16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="F16" s="5" t="n">
+        <v>109</v>
+      </c>
+      <c r="F16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="J16" s="5" t="n">
+        <v>109</v>
+      </c>
+      <c r="J16" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="N16" s="5" t="n">
+        <v>109</v>
+      </c>
+      <c r="N16" s="7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3145,43 +3395,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Retirement is now system level
- Rewrote the retirement process as a system level process instead of
  one running for each personnel member separately. Sets up nicely for
  changes of retirement regime for different states.
- Made some changes to the configuration Excel layout.
- Bugfix in the attrition process code.
</commit_message>
<xml_diff>
--- a/simParFile.xlsx
+++ b/simParFile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
     <sheet name="Attrition" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Retirement" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Output plots" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Misc" sheetId="10" state="hidden" r:id="rId11"/>
+    <sheet name="Misc" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -64,8 +64,118 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="E10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">1</t>
+        </r>
+        <r>
+          <rPr>
+            <vertAlign val="superscript"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">st</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> row: Computes the total weight of the distribution.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Other rows: Equals the cell above.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="E18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">1</t>
+        </r>
+        <r>
+          <rPr>
+            <vertAlign val="superscript"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">st</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> row: Computes the total weight of the distribution.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Other rows: Equals the cell above.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="122">
   <si>
     <t xml:space="preserve">General parameters</t>
   </si>
@@ -130,6 +240,12 @@
     <t xml:space="preserve">Years</t>
   </si>
   <si>
+    <t xml:space="preserve">Normalised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total weight</t>
+  </si>
+  <si>
     <t xml:space="preserve">M</t>
   </si>
   <si>
@@ -175,15 +291,15 @@
     <t xml:space="preserve">Initial state</t>
   </si>
   <si>
+    <t xml:space="preserve"># requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements</t>
+  </si>
+  <si>
     <t xml:space="preserve">Target # of personnel</t>
   </si>
   <si>
-    <t xml:space="preserve"># requirements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requirements</t>
-  </si>
-  <si>
     <t xml:space="preserve">Senior</t>
   </si>
   <si>
@@ -292,10 +408,13 @@
     <t xml:space="preserve">Name of recruitment type</t>
   </si>
   <si>
-    <t xml:space="preserve">Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test 2</t>
+    <t xml:space="preserve">Random</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adapt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix</t>
   </si>
   <si>
     <t xml:space="preserve">Time between recruitment cycles</t>
@@ -307,16 +426,22 @@
     <t xml:space="preserve">Fixed recruitment age?</t>
   </si>
   <si>
+    <t xml:space="preserve">Pointwise</t>
+  </si>
+  <si>
     <t xml:space="preserve">Piecewise Linear</t>
   </si>
   <si>
+    <t xml:space="preserve">Distribution nodes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amount</t>
   </si>
   <si>
     <t xml:space="preserve">Weight</t>
   </si>
   <si>
-    <t xml:space="preserve">Uniform</t>
+    <t xml:space="preserve">Piecewise Uniform</t>
   </si>
   <si>
     <t xml:space="preserve">Age in years</t>
@@ -395,6 +520,27 @@
   </si>
   <si>
     <t xml:space="preserve">Show percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS NOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;=</t>
   </si>
 </sst>
 </file>
@@ -407,7 +553,7 @@
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -444,6 +590,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -462,7 +622,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,8 +643,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor rgb="FFFFFF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFF66"/>
       </patternFill>
     </fill>
   </fills>
@@ -540,7 +706,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -573,7 +739,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -585,15 +763,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -609,7 +791,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -628,7 +810,13 @@
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
-    <dxf/>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+      </font>
+    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -637,7 +825,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFFF66"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -693,7 +881,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -704,10 +892,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0634230108757871"/>
-          <c:y val="0.0514973855173507"/>
-          <c:w val="0.898225529479107"/>
-          <c:h val="0.817778482015529"/>
+          <c:x val="0.0632911392405063"/>
+          <c:y val="0.0514869063470928"/>
+          <c:w val="0.89787760540592"/>
+          <c:h val="0.817280662819944"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -718,7 +906,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Recruitment!$C$24:$C$24</c:f>
+              <c:f>Recruitment!$C$25:$C$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -755,12 +943,12 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Recruitment!$B$25:$B$30</c:f>
+              <c:f>Recruitment!$B$26:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>19</c:v>
@@ -782,7 +970,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Recruitment!$C$25:$C$30</c:f>
+              <c:f>Recruitment!$C$26:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -809,11 +997,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="19853575"/>
-        <c:axId val="442317"/>
+        <c:axId val="15319353"/>
+        <c:axId val="30741354"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="19853575"/>
+        <c:axId val="15319353"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,12 +1036,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442317"/>
+        <c:crossAx val="30741354"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442317"/>
+        <c:axId val="30741354"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -897,7 +1085,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19853575"/>
+        <c:crossAx val="15319353"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -916,8 +1104,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.753080185821046"/>
-          <c:y val="0.161264946507237"/>
+          <c:x val="0.753054935713527"/>
+          <c:y val="0.161147203295833"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -948,14 +1136,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>33480</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>129960</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>129600</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>39960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -963,8 +1151,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33480" y="4950000"/>
-        <a:ext cx="3144240" cy="2271600"/>
+        <a:off x="33480" y="5112720"/>
+        <a:ext cx="3782160" cy="2432880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -985,14 +1173,14 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,11 +1264,11 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8" type="whole">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6" type="date">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6" type="date">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1101,27 +1289,72 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="n">
+      <c r="A1" s="22" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="n">
+      <c r="A2" s="22" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1140,19 +1373,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E30" activeCellId="0" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,21 +1445,43 @@
       <c r="C9" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>75</v>
       </c>
+      <c r="D10" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(C10),C10/E10,0)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <f aca="true">SUMIF(INDIRECT("C"&amp;(ROW())&amp;":C"&amp;(ROW()+B7-1)),"&gt; 0")</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>25</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(C11),C11/E11,0)</f>
+        <v>0.25</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <f aca="false">E10</f>
+        <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,7 +1489,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,21 +1526,43 @@
       <c r="C17" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>60</v>
       </c>
+      <c r="D18" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(C18),C18/E18,0)</f>
+        <v>0.6</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <f aca="true">SUMIF(INDIRECT("C"&amp;(ROW())&amp;":C"&amp;(ROW()+B15-1)),"&gt; 0")</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>40</v>
+      </c>
+      <c r="D19" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(C19),C19/E19,0)</f>
+        <v>0.4</v>
+      </c>
+      <c r="E19" s="9" t="n">
+        <f aca="false">E18</f>
+        <v>100</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,7 +1570,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,29 +1607,59 @@
       <c r="C25" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D25" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>10</v>
       </c>
+      <c r="D26" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(C26),C26/E26,0)</f>
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <f aca="true">SUMIF(INDIRECT("C"&amp;(ROW())&amp;":C"&amp;(ROW()+B23-1)),"&gt; 0")</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>30</v>
       </c>
+      <c r="D27" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(C27),C27/E27,0)</f>
+        <v>0.3</v>
+      </c>
+      <c r="E27" s="9" t="n">
+        <f aca="false">E26</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>60</v>
+      </c>
+      <c r="D28" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(C28),C28/E28,0)</f>
+        <v>0.6</v>
+      </c>
+      <c r="E28" s="9" t="n">
+        <f aca="false">E27</f>
+        <v>100</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1359,7 +1667,7 @@
         <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,21 +1704,43 @@
       <c r="C34" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D34" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>80</v>
       </c>
+      <c r="D35" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(C35),C35/E35,0)</f>
+        <v>0.8</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <f aca="true">SUMIF(INDIRECT("C"&amp;(ROW())&amp;":C"&amp;(ROW()+B32-1)),"&gt; 0")</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>20</v>
+      </c>
+      <c r="D36" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(C36),C36/E36,0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="E36" s="9" t="n">
+        <f aca="false">E35</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1434,6 +1764,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1444,28 +1775,29 @@
   </sheetPr>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="B32"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="B41" activeCellId="0" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>6</v>
@@ -1473,268 +1805,268 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="7" t="n">
+        <v>37</v>
+      </c>
+      <c r="B6" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="3" t="n">
-        <v>100</v>
+        <v>38</v>
+      </c>
+      <c r="B7" s="12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="B9" s="13" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="7" t="n">
+        <v>37</v>
+      </c>
+      <c r="B12" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>100</v>
+        <v>38</v>
+      </c>
+      <c r="B13" s="12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="3" t="n">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="B15" s="13" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="7" t="n">
+        <v>37</v>
+      </c>
+      <c r="B18" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="3" t="n">
-        <v>100</v>
+        <v>38</v>
+      </c>
+      <c r="B19" s="12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="3" t="n">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="B21" s="13" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="7" t="n">
+        <v>37</v>
+      </c>
+      <c r="B24" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="3" t="n">
-        <v>100</v>
+        <v>38</v>
+      </c>
+      <c r="B25" s="12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="3" t="n">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
+      </c>
+      <c r="B27" s="13" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="7" t="n">
+        <v>37</v>
+      </c>
+      <c r="B30" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="3" t="n">
-        <v>100</v>
+        <v>38</v>
+      </c>
+      <c r="B31" s="12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="3" t="n">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="B33" s="13" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="7" t="n">
+        <v>37</v>
+      </c>
+      <c r="B36" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3" t="n">
-        <v>-1</v>
+        <v>38</v>
+      </c>
+      <c r="B37" s="12" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="3" t="n">
-        <v>2</v>
+        <v>39</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>21</v>
+      <c r="B39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>22</v>
+      <c r="A40" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="13" t="n">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -1742,7 +2074,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B8 B14 B20 B26 B32 B38" type="whole">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3 B7 B13 B19 B25 B31 B37" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1750,11 +2082,11 @@
       <formula1>Misc!$A$1:$A$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B9:C9 B15:C15 B21:C21 B27:C27 B33:C33 B39:C40" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B8:C8 B14:C14 B20:C20 B26:C26 B32:C32 B38:C39" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7 B13 B19 B25 B31 B37" type="whole">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9 B15 B21 B27 B33 B40" type="whole">
       <formula1>-1</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1777,28 +2109,29 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
-      <selection pane="bottomRight" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>3</v>
@@ -1806,387 +2139,387 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="9" t="n">
+        <v>52</v>
+      </c>
+      <c r="B8" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="9" t="n">
+        <v>53</v>
+      </c>
+      <c r="B9" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="10" t="n">
+        <v>54</v>
+      </c>
+      <c r="B10" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="B11" s="14" t="n">
         <v>0</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="B12" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="B13" s="14" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="12" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" s="16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="10" t="n">
+        <v>61</v>
+      </c>
+      <c r="B15" s="14" t="n">
         <v>10</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="10" t="n">
+        <v>63</v>
+      </c>
+      <c r="B16" s="14" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="13" t="n">
+        <v>64</v>
+      </c>
+      <c r="B17" s="17" t="n">
         <v>0.25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="13" t="n">
+      <c r="B18" s="17" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>63</v>
+        <v>48</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>39</v>
+        <v>50</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="9" t="n">
+        <v>52</v>
+      </c>
+      <c r="B23" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="9" t="n">
+        <v>53</v>
+      </c>
+      <c r="B24" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="10" t="n">
+        <v>54</v>
+      </c>
+      <c r="B25" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="B26" s="14" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="B27" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="B28" s="14" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="12" t="n">
+        <v>60</v>
+      </c>
+      <c r="B29" s="16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="10" t="n">
+        <v>61</v>
+      </c>
+      <c r="B30" s="14" t="n">
         <v>10</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="10" t="n">
+        <v>63</v>
+      </c>
+      <c r="B31" s="14" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="13" t="n">
+        <v>64</v>
+      </c>
+      <c r="B32" s="17" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="13" t="n">
+      <c r="B33" s="17" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>64</v>
+        <v>48</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>31</v>
+        <v>50</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="9" t="n">
+        <v>52</v>
+      </c>
+      <c r="B38" s="12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D39" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>27</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40" s="9" t="n">
+        <v>53</v>
+      </c>
+      <c r="B40" s="12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>26</v>
+        <v>69</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="10" t="n">
+        <v>54</v>
+      </c>
+      <c r="B42" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="B43" s="14" t="n">
         <v>0</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B44" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="B44" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="B45" s="14" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="12" t="n">
+        <v>60</v>
+      </c>
+      <c r="B46" s="16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="10" t="n">
+        <v>61</v>
+      </c>
+      <c r="B47" s="14" t="n">
         <v>5</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" s="10" t="n">
+        <v>63</v>
+      </c>
+      <c r="B48" s="14" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B49" s="13" t="n">
+        <v>64</v>
+      </c>
+      <c r="B49" s="17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2194,21 +2527,17 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations count="12">
+  <dataValidations count="11">
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:B7 B20:B22 B35:B37" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:B7 B20:B22 B35:B37 D39 B41:C41" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B14 B29 B46" type="list">
-      <formula1>Misc!$A$1:$A$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C12 C27 C44" type="list">
-      <formula1>"years,months"</formula1>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8:B9 B23:B24 B38 B40" type="whole">
+      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10 B12 B25 B27 B42 B44" type="decimal">
@@ -2219,6 +2548,18 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C12 C27 C44" type="list">
+      <formula1>"years,months"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B13 B15 B28 B30 B45 B47" type="whole">
+      <formula1>-1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B14 B29 B46" type="list">
+      <formula1>Misc!$A$1:$A$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B16 B31 B48" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
@@ -2227,20 +2568,8 @@
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B13 B15 B28 B30 B45 B47" type="whole">
-      <formula1>-1</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8:B9 B23:B24 B38 B40" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C39" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C39" type="list">
       <formula1>Misc!$C$1:$C$8</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D39 B41:C41" type="none">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2262,20 +2591,25 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>1</v>
@@ -2283,7 +2617,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>4</v>
@@ -2291,25 +2625,25 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2347,418 +2681,971 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="O22" activeCellId="0" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>76</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="3" t="n">
+        <v>55</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>53</v>
+      <c r="H6" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="3" t="n">
+        <v>55</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>53</v>
+      <c r="M7" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="str">
+      <c r="A8" s="18" t="str">
         <f aca="false">IF(B10,"Min recruitment","ignored")</f>
         <v>ignored</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>92</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14" t="str">
-        <f aca="false">IF(F10,"Min recruitment","ignored")</f>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18" t="str">
+        <f aca="false">IF(G10,"Min recruitment","ignored")</f>
         <v>Min recruitment</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="G8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="18" t="str">
+        <f aca="false">IF(L10,"Min recruitment","ignored")</f>
+        <v>ignored</v>
+      </c>
+      <c r="L8" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="M8" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="str">
+      <c r="A9" s="18" t="str">
         <f aca="false">IF(B10,"Max recruitment",IF(B11,"ignored","Recruitment"))</f>
         <v>ignored</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14" t="str">
-        <f aca="false">IF(F10,"Max recruitment",IF(F11,"ignored","Recruitment"))</f>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18" t="str">
+        <f aca="false">IF(G10,"Max recruitment",IF(G11,"ignored","Recruitment"))</f>
         <v>Max recruitment</v>
       </c>
-      <c r="F9" s="3" t="n">
-        <v>55</v>
-      </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="3" t="n">
+        <v>175</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="18" t="str">
+        <f aca="false">IF(L10,"Max recruitment",IF(L11,"ignored","Recruitment"))</f>
+        <v>Recruitment</v>
+      </c>
+      <c r="L9" s="3" t="n">
+        <v>140</v>
+      </c>
+      <c r="M9" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="7" t="n">
-        <v>1</v>
+      <c r="F10" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="str">
+      <c r="A11" s="18" t="str">
         <f aca="false">IF(B10,"ignored","Random recruitment")</f>
         <v>Random recruitment</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="14" t="str">
-        <f aca="false">IF(F10,"ignored","Random recruitment")</f>
+      <c r="F11" s="18" t="str">
+        <f aca="false">IF(G10,"ignored","Random recruitment")</f>
         <v>ignored</v>
       </c>
-      <c r="F11" s="7" t="n">
-        <v>1</v>
+      <c r="G11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18" t="str">
+        <f aca="false">IF(L10,"ignored","Random recruitment")</f>
+        <v>Random recruitment</v>
+      </c>
+      <c r="L11" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B12" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="7" t="n">
+      <c r="F12" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="L12" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="str">
+      <c r="A13" s="18" t="str">
         <f aca="false">IF(B12,"Recruitment age","ignored")</f>
         <v>ignored</v>
       </c>
       <c r="B13" s="3" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18" t="str">
+        <f aca="false">IF(G12,"Recruitment age","ignored")</f>
+        <v>ignored</v>
+      </c>
+      <c r="G13" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="H13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="str">
-        <f aca="false">IF(F12,"Recruitment age","ignored")</f>
+      <c r="K13" s="18" t="str">
+        <f aca="false">IF(L12,"Recruitment age","ignored")</f>
         <v>ignored</v>
       </c>
-      <c r="F13" s="3" t="n">
+      <c r="L13" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="M13" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="str">
+      <c r="A15" s="18" t="str">
         <f aca="false">IF(AND(NOT(B10),B11),"# of recruits distribution","ignored")</f>
         <v># of recruits distribution</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14" t="str">
-        <f aca="false">IF(AND(NOT(F10),F11),"# of recruits distribution","ignored")</f>
+        <v>83</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18" t="str">
+        <f aca="false">IF(AND(NOT(G10),G11),"# of recruits distribution","ignored")</f>
         <v>ignored</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="14"/>
+      <c r="G15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="18"/>
+      <c r="K15" s="18" t="str">
+        <f aca="false">IF(AND(NOT(L10),L11),"# of recruits distribution","ignored")</f>
+        <v>ignored</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>82</v>
-      </c>
+      <c r="A16" s="18" t="str">
+        <f aca="false">IF(AND(NOT(B10),B11),"# of distribution nodes","ignored")</f>
+        <v># of distribution nodes</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18" t="str">
+        <f aca="false">IF(AND(NOT(G10),G11),"# of distribution nodes","ignored")</f>
+        <v>ignored</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="K16" s="18" t="str">
+        <f aca="false">IF(AND(NOT(L10),L11),"# of distribution nodes","ignored")</f>
+        <v>ignored</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="M16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2" t="n">
-        <v>35</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>3</v>
+      <c r="A17" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="0" t="str">
+        <f aca="false">IF(B15="Pointwise","Normalised","")</f>
+        <v>Normalised</v>
+      </c>
+      <c r="E17" s="0" t="str">
+        <f aca="false">IF(B15="Pointwise","Total weight","")</f>
+        <v>Total weight</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="0" t="str">
+        <f aca="false">IF(G15="Pointwise","Normalised","")</f>
+        <v/>
+      </c>
+      <c r="J17" s="0" t="str">
+        <f aca="false">IF(G15="Pointwise","Total weight","")</f>
+        <v/>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M17" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="N17" s="0" t="str">
+        <f aca="false">IF(L15="Pointwise","Normalised","")</f>
+        <v/>
+      </c>
+      <c r="O17" s="0" t="str">
+        <f aca="false">IF(L15="Pointwise","Total weight","")</f>
+        <v/>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="n">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="C18" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="D18" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(E18),IF(ISNUMBER(C18),C18/E18,0),"")</f>
+        <v>0.25</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <f aca="true">IF(B15="Pointwise",SUMIF(INDIRECT("C"&amp;(ROW())&amp;":C"&amp;(ROW()+B16-1)),"&gt; 0"),"")</f>
+        <v>100</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="H18" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="F18" s="2" t="n">
-        <v>95</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>1</v>
+      <c r="I18" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(J18),IF(ISNUMBER(H18),H18/J18,0),"")</f>
+        <v/>
+      </c>
+      <c r="J18" s="0" t="str">
+        <f aca="true">IF(G15="Pointwise",SUMIF(INDIRECT("C"&amp;(ROW())&amp;":C"&amp;(ROW()+G16-1)),"&gt; 0"),"")</f>
+        <v/>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="N18" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(O18),IF(ISNUMBER(M18),M18/O18,0),"")</f>
+        <v/>
+      </c>
+      <c r="O18" s="0" t="str">
+        <f aca="true">IF(L15="Pointwise",SUMIF(INDIRECT("C"&amp;(ROW())&amp;":C"&amp;(ROW()+L16-1)),"&gt; 0"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="n">
-        <v>55</v>
+        <v>140</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D19" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(E19),IF(ISNUMBER(C19),C19/E19,0),"")</f>
+        <v>0.2</v>
+      </c>
+      <c r="E19" s="9" t="n">
+        <f aca="false">E18</f>
         <v>100</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>0</v>
+        <v>95</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(J19),IF(ISNUMBER(H19),H19/J19,0),"")</f>
+        <v/>
+      </c>
+      <c r="J19" s="9" t="str">
+        <f aca="false">J18</f>
+        <v/>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(O19),IF(ISNUMBER(M19),M19/O19,0),"")</f>
+        <v/>
+      </c>
+      <c r="O19" s="9" t="str">
+        <f aca="false">O18</f>
+        <v/>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="F20" s="2" t="n">
+      <c r="B20" s="2" t="n">
+        <v>160</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="D20" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(E20),IF(ISNUMBER(C20),C20/E20,0),"")</f>
+        <v>0.3</v>
+      </c>
+      <c r="E20" s="9" t="n">
+        <f aca="false">E19</f>
+        <v>100</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(J20),IF(ISNUMBER(H20),H20/J20,0),"")</f>
+        <v/>
+      </c>
+      <c r="J20" s="9" t="str">
+        <f aca="false">J19</f>
+        <v/>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(O20),IF(ISNUMBER(M20),M20/O20,0),"")</f>
+        <v/>
+      </c>
+      <c r="O20" s="9" t="str">
+        <f aca="false">O19</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="2" t="n">
+        <v>175</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="D21" s="8" t="n">
+        <f aca="false">IF(ISNUMBER(E21),IF(ISNUMBER(C21),C21/E21,0),"")</f>
+        <v>0.25</v>
+      </c>
+      <c r="E21" s="9" t="n">
+        <f aca="false">E20</f>
+        <v>100</v>
+      </c>
+      <c r="G21" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="G20" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="F21" s="2" t="n">
+      <c r="H21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(J21),IF(ISNUMBER(H21),H21/J21,0),"")</f>
+        <v/>
+      </c>
+      <c r="J21" s="9" t="str">
+        <f aca="false">J20</f>
+        <v/>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="M21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(O21),IF(ISNUMBER(M21),M21/O21,0),"")</f>
+        <v/>
+      </c>
+      <c r="O21" s="9" t="str">
+        <f aca="false">O20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="2" t="n">
         <v>110</v>
       </c>
-      <c r="G21" s="2" t="n">
+      <c r="H22" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I22" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(J22),IF(ISNUMBER(H22),H22/J22,0),"")</f>
+        <v/>
+      </c>
+      <c r="J22" s="9" t="str">
+        <f aca="false">J21</f>
+        <v/>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="M22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="N22" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(O22),IF(ISNUMBER(M22),M22/O22,0),"")</f>
+        <v/>
+      </c>
+      <c r="O22" s="9" t="str">
+        <f aca="false">O21</f>
+        <v/>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="str">
-        <f aca="false">IF(B12,"ignored","Recruitment age distribution")</f>
+      <c r="A23" s="18" t="str">
+        <f aca="false">IF(B$12,"ignored","Recruitment age distribution")</f>
         <v>Recruitment age distribution</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14" t="str">
-        <f aca="false">IF(F12,"ignored","Recruitment age distribution")</f>
+        <v>88</v>
+      </c>
+      <c r="C23" s="18"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="18" t="str">
+        <f aca="false">IF(B$12,"ignored","# of distribution nodes")</f>
+        <v># of distribution nodes</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18" t="str">
+        <f aca="false">IF(G$12,"ignored","Recruitment age distribution")</f>
         <v>Recruitment age distribution</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="F24" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>82</v>
-      </c>
+      <c r="G24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="18"/>
+      <c r="K24" s="18" t="str">
+        <f aca="false">IF(L$12,"ignored","Recruitment age distribution")</f>
+        <v>Recruitment age distribution</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M24" s="18"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F25" s="2" t="n">
-        <v>18</v>
+      <c r="A25" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="0" t="str">
+        <f aca="false">IF(B23="Pointwise","Normalised","")</f>
+        <v/>
+      </c>
+      <c r="E25" s="0" t="str">
+        <f aca="false">IF(B23="Pointwise","Total weight","")</f>
+        <v/>
+      </c>
+      <c r="F25" s="18" t="str">
+        <f aca="false">IF(G$12,"ignored","# of distribution nodes")</f>
+        <v># of distribution nodes</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="H25" s="18"/>
+      <c r="K25" s="18" t="str">
+        <f aca="false">IF(L$12,"ignored","# of distribution nodes")</f>
+        <v># of distribution nodes</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="M25" s="18"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="n">
-        <v>19</v>
+        <v>18.5</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="F26" s="2" t="n">
-        <v>19</v>
-      </c>
-      <c r="G26" s="2" t="n">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="D26" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(E26),IF(ISNUMBER(C26),C26/E26,0),"")</f>
+        <v/>
+      </c>
+      <c r="E26" s="0" t="str">
+        <f aca="true">IF(B23="Pointwise",SUMIF(INDIRECT("C"&amp;(ROW())&amp;":C"&amp;(ROW()+B24-1)),"&gt; 0"),"")</f>
+        <v/>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="0" t="str">
+        <f aca="false">IF(G24="Pointwise","Normalised","")</f>
+        <v/>
+      </c>
+      <c r="J26" s="0" t="str">
+        <f aca="false">IF(G24="Pointwise","Total weight","")</f>
+        <v/>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="L26" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="M26" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="N26" s="0" t="str">
+        <f aca="false">IF(L24="Pointwise","Normalised","")</f>
+        <v/>
+      </c>
+      <c r="O26" s="0" t="str">
+        <f aca="false">IF(L24="Pointwise","Total weight","")</f>
+        <v/>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="F27" s="2" t="n">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="D27" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(E27),IF(ISNUMBER(C27),C27/E27,0),"")</f>
+        <v/>
+      </c>
+      <c r="E27" s="9" t="str">
+        <f aca="false">E26</f>
+        <v/>
       </c>
       <c r="G27" s="2" t="n">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="I27" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(J27),IF(ISNUMBER(H27),H27/J27,0),"")</f>
+        <v/>
+      </c>
+      <c r="J27" s="0" t="str">
+        <f aca="true">IF(G24="Pointwise",SUMIF(INDIRECT("C"&amp;(ROW())&amp;":C"&amp;(ROW()+G25-1)),"&gt; 0"),"")</f>
+        <v/>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="M27" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="N27" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(O27),IF(ISNUMBER(M27),M27/O27,0),"")</f>
+        <v/>
+      </c>
+      <c r="O27" s="0" t="str">
+        <f aca="true">IF(L24="Pointwise",SUMIF(INDIRECT("C"&amp;(ROW())&amp;":C"&amp;(ROW()+L25-1)),"&gt; 0"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="F28" s="2" t="n">
-        <v>21</v>
+        <v>4</v>
+      </c>
+      <c r="D28" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(E28),IF(ISNUMBER(C28),C28/E28,0),"")</f>
+        <v/>
+      </c>
+      <c r="E28" s="9" t="str">
+        <f aca="false">E27</f>
+        <v/>
       </c>
       <c r="G28" s="2" t="n">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="I28" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(J28),IF(ISNUMBER(H28),H28/J28,0),"")</f>
+        <v/>
+      </c>
+      <c r="J28" s="9" t="str">
+        <f aca="false">J27</f>
+        <v/>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="M28" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="N28" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(O28),IF(ISNUMBER(M28),M28/O28,0),"")</f>
+        <v/>
+      </c>
+      <c r="O28" s="9" t="str">
+        <f aca="false">O27</f>
+        <v/>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2" t="n">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="D29" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(E29),IF(ISNUMBER(C29),C29/E29,0),"")</f>
+        <v/>
+      </c>
+      <c r="E29" s="9" t="str">
+        <f aca="false">E28</f>
+        <v/>
       </c>
       <c r="G29" s="2" t="n">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I29" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(J29),IF(ISNUMBER(H29),H29/J29,0),"")</f>
+        <v/>
+      </c>
+      <c r="J29" s="9" t="str">
+        <f aca="false">J28</f>
+        <v/>
+      </c>
+      <c r="L29" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M29" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="N29" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(O29),IF(ISNUMBER(M29),M29/O29,0),"")</f>
+        <v/>
+      </c>
+      <c r="O29" s="9" t="str">
+        <f aca="false">O28</f>
+        <v/>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(E30),IF(ISNUMBER(C30),C30/E30,0),"")</f>
+        <v/>
+      </c>
+      <c r="E30" s="9" t="str">
+        <f aca="false">E29</f>
+        <v/>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I30" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(J30),IF(ISNUMBER(H30),H30/J30,0),"")</f>
+        <v/>
+      </c>
+      <c r="J30" s="9" t="str">
+        <f aca="false">J29</f>
+        <v/>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="M30" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="N30" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(O30),IF(ISNUMBER(M30),M30/O30,0),"")</f>
+        <v/>
+      </c>
+      <c r="O30" s="9" t="str">
+        <f aca="false">O29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="C30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2" t="n">
+      <c r="C31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(E31),IF(ISNUMBER(C31),C31/E31,0),"")</f>
+        <v/>
+      </c>
+      <c r="E31" s="9" t="str">
+        <f aca="false">E30</f>
+        <v/>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I31" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(J31),IF(ISNUMBER(H31),H31/J31,0),"")</f>
+        <v/>
+      </c>
+      <c r="J31" s="9" t="str">
+        <f aca="false">J30</f>
+        <v/>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="M31" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="N31" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(O31),IF(ISNUMBER(M31),M31/O31,0),"")</f>
+        <v/>
+      </c>
+      <c r="O31" s="9" t="str">
+        <f aca="false">O30</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="G30" s="2" t="n">
-        <v>0</v>
+      <c r="H32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(J32),IF(ISNUMBER(H32),H32/J32,0),"")</f>
+        <v/>
+      </c>
+      <c r="J32" s="9" t="str">
+        <f aca="false">J31</f>
+        <v/>
+      </c>
+      <c r="L32" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="M32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" s="8" t="str">
+        <f aca="false">IF(ISNUMBER(O32),IF(ISNUMBER(M32),M32/O32,0),"")</f>
+        <v/>
+      </c>
+      <c r="O32" s="9" t="str">
+        <f aca="false">O31</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -2766,36 +3653,36 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10:B12 F10:F12" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10:B12 G10:G12 L10:L12" type="list">
       <formula1>Misc!$A$1:$A$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 F6" type="decimal">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B13 F13" type="decimal">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B23 F23" type="list">
-      <formula1>"Pointwise,Uniform"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7 F7" type="decimal">
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6 G6 L6" type="decimal">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8:B9 F8:F9" type="decimal">
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7 G7 L7" type="decimal">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B15 F15" type="list">
-      <formula1>"Pointwise,Uniform,Piecewise Linear"</formula1>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8:B9 G8:G9 L8:L9" type="decimal">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B13 G13 L13" type="decimal">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B16 G16 L16 B24 G25 L25" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B15 G15 L15 B23 G24 L24" type="list">
+      <formula1>Misc!$B$1:$B$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2806,7 +3693,8 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2818,83 +3706,83 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="str">
+      <c r="A5" s="18" t="str">
         <f aca="false">IF(B4,"Probability of attrition/period","ignored")</f>
         <v>ignored</v>
       </c>
-      <c r="B5" s="15" t="n">
+      <c r="B5" s="19" t="n">
         <v>0.02</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="str">
+      <c r="A7" s="18" t="str">
         <f aca="false">IF(B4,"ignored","Attrition rate")</f>
         <v>Attrition rate</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>88</v>
+      <c r="C7" s="18" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="15" t="n">
-        <v>0.01</v>
+      <c r="C8" s="19" t="n">
+        <v>0.02</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="15" t="n">
-        <v>0.0075</v>
+      <c r="C9" s="19" t="n">
+        <v>0.015</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="C10" s="15" t="n">
-        <v>0.005</v>
+      <c r="C10" s="19" t="n">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
@@ -2948,41 +3836,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>45</v>
@@ -2993,7 +3881,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>67</v>
@@ -3037,30 +3925,31 @@
   </sheetPr>
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>93</v>
+      <c r="A1" s="20" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>95</v>
+      <c r="A3" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>100</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>0</v>
@@ -3068,87 +3957,87 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="J5" s="2"/>
       <c r="M5" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="J6" s="3" t="n">
         <v>6</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="N6" s="3" t="n">
         <v>12</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F7" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="J7" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="N7" s="7" t="n">
         <v>1</v>
@@ -3156,25 +4045,25 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="N8" s="7" t="n">
         <v>1</v>
@@ -3182,25 +4071,25 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F9" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="J9" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="N9" s="7" t="n">
         <v>1</v>
@@ -3208,25 +4097,25 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F10" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J10" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="N10" s="7" t="n">
         <v>1</v>
@@ -3234,61 +4123,61 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F12" s="2"/>
       <c r="I12" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="N12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B13" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F13" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="J13" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="N13" s="7" t="n">
         <v>1</v>
@@ -3296,25 +4185,25 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B14" s="7" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F14" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="J14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="N14" s="7" t="n">
         <v>1</v>
@@ -3322,25 +4211,25 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="J15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="N15" s="7" t="n">
         <v>1</v>
@@ -3348,25 +4237,25 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="J16" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="N16" s="7" t="n">
         <v>1</v>
@@ -3374,16 +4263,16 @@
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F5 J5 N5 B12 F12 J12 N12" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F3 B6 F6 J6 N6" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B7:B10 F7:F10 J7:J10 N7:N10 B13:B16 F13:F16 J13:J16 N13:N16" type="list">
       <formula1>Misc!$A$1:$A$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F5 J5 N5 B12 F12 J12 N12" type="none">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Overhaul of attrition logic (v0.5.0)
- Overhauled the internal logic of attrition handling to allow different
  attrition schemes for different states. Bonus: attrition logic is also
  significantly faster.
- Added option to retirement such that user can choose whether
  retirement happens when either condition (age or tenure) or both
  conditions are satisfied.
</commit_message>
<xml_diff>
--- a/simParFile.xlsx
+++ b/simParFile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -125,6 +125,21 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="B15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">* Pointwise: only the listed values are possible.
+* Piecewise Uniform: interval randomly chosen based on entered weights, then uniformly random within interval (endpoint excluded). Weight of point with highest value gets ignored.
+* Piecewise Linear: density function is (normalization of) linear interpolation between entered  points and weights.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E18" authorId="0">
       <text>
         <r>
@@ -553,7 +568,7 @@
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -602,17 +617,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -791,7 +795,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -834,7 +838,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -868,7 +872,7 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -879,290 +883,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0632911392405063"/>
-          <c:y val="0.0514869063470928"/>
-          <c:w val="0.89787760540592"/>
-          <c:h val="0.817280662819944"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Recruitment!$C$25:$C$25</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Weight</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Recruitment!$B$26:$B$31</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>18.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Recruitment!$C$26:$C$31</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="15319353"/>
-        <c:axId val="30741354"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="15319353"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="30741354"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="30741354"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="15319353"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.753054935713527"/>
-          <c:y val="0.161147203295833"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>33480</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>39960</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="33480" y="5112720"/>
-        <a:ext cx="3782160" cy="2432880"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1178,9 +898,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,13 +1011,13 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,8 +1105,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,18 +1494,17 @@
   </sheetPr>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="B41" activeCellId="0" sqref="B41"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2109,18 +1827,18 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
       <selection pane="bottomRight" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2596,9 +2314,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2688,19 +2405,19 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O22" activeCellId="0" sqref="O22"/>
+      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3693,8 +3410,7 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3711,8 +3427,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3836,8 +3552,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3935,8 +3651,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>